<commit_message>
Fixed XLSX file, some styling, linked header, and first pass at templating out metadata sources.
</commit_message>
<xml_diff>
--- a/test/data/HOLLIS_Links_013696939.xlsx
+++ b/test/data/HOLLIS_Links_013696939.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="300" windowWidth="16500" windowHeight="11820"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Call No:</t>
   </si>
@@ -64,16 +64,19 @@
   </si>
   <si>
     <t>http://hollis.harvard.edu/?itemid=|library/m/aleph|013696939</t>
+  </si>
+  <si>
+    <t>http://nrs.harvard.edu/urn-3:RAD.SCHL:13212733</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,16 +91,317 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -105,15 +409,163 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -139,13 +591,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -224,6 +723,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -258,6 +758,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,29 +934,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -463,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -471,7 +972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -479,33 +980,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" s="7" customFormat="1">
+      <c r="B8" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="7" customFormat="1">
+      <c r="B9" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -513,7 +1016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="7" customFormat="1">
+    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -521,66 +1024,67 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="7" customFormat="1">
+    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12"/>
-    </row>
-    <row r="13" spans="1:2" s="7" customFormat="1">
+      <c r="C12"/>
+    </row>
+    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13"/>
     </row>
-    <row r="14" spans="1:2" s="7" customFormat="1">
+    <row r="14" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:2" s="7" customFormat="1">
+    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:2" s="7" customFormat="1">
+    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:3" s="7" customFormat="1">
+    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="2"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="2"/>
     </row>
@@ -595,24 +1099,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>